<commit_message>
ALL TEST CASES PASSED
</commit_message>
<xml_diff>
--- a/Test Cases.xlsx
+++ b/Test Cases.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="15600" yWindow="460" windowWidth="10000" windowHeight="14720" tabRatio="500"/>
+    <workbookView xWindow="12560" yWindow="460" windowWidth="13040" windowHeight="14720" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -289,18 +289,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -315,12 +309,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -329,6 +319,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -608,8 +601,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F76"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -622,16 +615,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="19" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2" t="s">
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -985,13 +978,13 @@
       <c r="B20" t="s">
         <v>24</v>
       </c>
-      <c r="C20" s="1">
-        <v>0</v>
+      <c r="C20" s="4">
+        <v>1</v>
       </c>
       <c r="E20" t="s">
         <v>14</v>
       </c>
-      <c r="F20" s="6">
+      <c r="F20" s="4">
         <v>1</v>
       </c>
     </row>
@@ -1082,8 +1075,8 @@
       <c r="B25" t="s">
         <v>16</v>
       </c>
-      <c r="C25" s="1">
-        <v>0</v>
+      <c r="C25" s="4">
+        <v>1</v>
       </c>
       <c r="D25" t="s">
         <v>37</v>
@@ -1265,16 +1258,16 @@
       </c>
     </row>
     <row r="39" spans="1:6" ht="19" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
+      <c r="A39" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="B39" s="2"/>
-      <c r="C39" s="2"/>
-      <c r="D39" s="2" t="s">
+      <c r="B39" s="5"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="E39" s="2"/>
-      <c r="F39" s="2"/>
+      <c r="E39" s="5"/>
+      <c r="F39" s="5"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
@@ -1300,7 +1293,7 @@
       <c r="B41" t="s">
         <v>14</v>
       </c>
-      <c r="E41" s="3" t="s">
+      <c r="E41" s="1" t="s">
         <v>69</v>
       </c>
       <c r="F41">
@@ -1320,7 +1313,7 @@
       <c r="D42" t="s">
         <v>13</v>
       </c>
-      <c r="E42" s="5" t="s">
+      <c r="E42" s="3" t="s">
         <v>16</v>
       </c>
       <c r="F42">
@@ -1340,7 +1333,7 @@
       <c r="D43" t="s">
         <v>37</v>
       </c>
-      <c r="E43" s="5" t="s">
+      <c r="E43" s="3" t="s">
         <v>70</v>
       </c>
       <c r="F43">
@@ -1360,7 +1353,7 @@
       <c r="D44" t="s">
         <v>13</v>
       </c>
-      <c r="E44" s="5" t="s">
+      <c r="E44" s="3" t="s">
         <v>16</v>
       </c>
       <c r="F44">
@@ -1380,7 +1373,7 @@
       <c r="D45" t="s">
         <v>4</v>
       </c>
-      <c r="E45" s="5" t="s">
+      <c r="E45" s="3" t="s">
         <v>30</v>
       </c>
       <c r="F45">
@@ -1400,7 +1393,7 @@
       <c r="D46" t="s">
         <v>67</v>
       </c>
-      <c r="E46" s="5" t="s">
+      <c r="E46" s="3" t="s">
         <v>69</v>
       </c>
       <c r="F46">
@@ -1420,7 +1413,7 @@
       <c r="D47" t="s">
         <v>4</v>
       </c>
-      <c r="E47" s="5" t="s">
+      <c r="E47" s="3" t="s">
         <v>71</v>
       </c>
       <c r="F47">
@@ -1440,7 +1433,7 @@
       <c r="D48" t="s">
         <v>67</v>
       </c>
-      <c r="E48" s="5" t="s">
+      <c r="E48" s="3" t="s">
         <v>72</v>
       </c>
       <c r="F48">
@@ -1457,7 +1450,7 @@
       <c r="D49" t="s">
         <v>4</v>
       </c>
-      <c r="E49" s="5" t="s">
+      <c r="E49" s="3" t="s">
         <v>73</v>
       </c>
       <c r="F49">
@@ -1474,7 +1467,7 @@
       <c r="D50" t="s">
         <v>68</v>
       </c>
-      <c r="E50" s="5" t="s">
+      <c r="E50" s="3" t="s">
         <v>74</v>
       </c>
       <c r="F50">
@@ -1494,7 +1487,7 @@
       <c r="D51" t="s">
         <v>4</v>
       </c>
-      <c r="E51" s="5" t="s">
+      <c r="E51" s="3" t="s">
         <v>75</v>
       </c>
       <c r="F51">
@@ -1514,7 +1507,7 @@
       <c r="D52" t="s">
         <v>4</v>
       </c>
-      <c r="E52" s="5" t="s">
+      <c r="E52" s="3" t="s">
         <v>30</v>
       </c>
       <c r="F52">
@@ -1534,7 +1527,7 @@
       <c r="D53" t="s">
         <v>37</v>
       </c>
-      <c r="E53" s="5" t="s">
+      <c r="E53" s="3" t="s">
         <v>71</v>
       </c>
       <c r="F53">
@@ -1545,7 +1538,7 @@
       <c r="D54" t="s">
         <v>67</v>
       </c>
-      <c r="E54" s="5" t="s">
+      <c r="E54" s="3" t="s">
         <v>72</v>
       </c>
       <c r="F54">
@@ -1556,7 +1549,7 @@
       <c r="D55" t="s">
         <v>13</v>
       </c>
-      <c r="E55" s="5" t="s">
+      <c r="E55" s="3" t="s">
         <v>31</v>
       </c>
       <c r="F55">
@@ -1564,11 +1557,11 @@
       </c>
     </row>
     <row r="57" spans="1:6" ht="19" x14ac:dyDescent="0.25">
-      <c r="A57" s="2" t="s">
+      <c r="A57" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="B57" s="2"/>
-      <c r="C57" s="2"/>
+      <c r="B57" s="5"/>
+      <c r="C57" s="5"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
@@ -1590,7 +1583,7 @@
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A60" s="4" t="s">
+      <c r="A60" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B60" t="s">

</xml_diff>